<commit_message>
Application on Face Recognition
</commit_message>
<xml_diff>
--- a/data/Face_recognition.xlsx
+++ b/data/Face_recognition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacMini2/france/francesco/Dropbox/Interval_data_project/Dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alfo/Dropbox/Interval_data_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E726AC7-63A0-594F-9CB9-874A57D7A6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{630B66D6-1F3E-D844-AE5B-AC3526B746A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10360" yWindow="4160" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dati Viviana" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -667,9 +667,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2187,7 +2187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:M28"/>
     </sheetView>
   </sheetViews>
@@ -3347,7 +3347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45E2D02-AA52-A44D-975D-C0559F05439D}">
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>

</xml_diff>